<commit_message>
feat: modal add props chore: scss
</commit_message>
<xml_diff>
--- a/src/i18n/i18n_table.xlsx
+++ b/src/i18n/i18n_table.xlsx
@@ -24,11 +24,11 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="篩選器 2" guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="AJ篩選 非本人勿用" guid="{26C905C7-2C39-4702-9479-6A8F4386ED3B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 3" guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 4" guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 1" guid="{38507902-7545-485C-834F-5E4850BE1025}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="篩選器 2" guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="367">
   <si>
     <t>Key</t>
   </si>
@@ -166,18 +166,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>ExcelSystem</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExcelTest</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExcelPage</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Excel系統123</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1367,6 +1355,65 @@
   </si>
   <si>
     <t>Save</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ccolor Tone</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel Page</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel Test</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel System</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>色调</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorTone</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>light</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>dark</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dark</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>色調</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>深色
+色調</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>浅色
+色調</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>淺色
+色調</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1467,7 +1514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1557,11 +1604,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1584,11 +1666,50 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1862,8 +1983,8 @@
   <dimension ref="A1:U106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E96" sqref="E96:H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -2024,16 +2145,16 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2057,16 +2178,16 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -2092,16 +2213,16 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -2127,16 +2248,16 @@
         <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2160,16 +2281,16 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2195,16 +2316,16 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2230,16 +2351,16 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2263,16 +2384,16 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2296,16 +2417,16 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2329,16 +2450,16 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2362,16 +2483,16 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2395,16 +2516,16 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2428,16 +2549,16 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2461,16 +2582,16 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2494,16 +2615,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2527,16 +2648,16 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2560,16 +2681,16 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2593,16 +2714,16 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2625,16 +2746,16 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1">
@@ -2644,16 +2765,16 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1">
@@ -2663,16 +2784,16 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1">
@@ -2682,16 +2803,16 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15" customHeight="1">
@@ -2701,16 +2822,16 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1">
@@ -2720,16 +2841,16 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15" customHeight="1">
@@ -2739,16 +2860,16 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15" customHeight="1">
@@ -2758,16 +2879,16 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1">
@@ -2777,16 +2898,16 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1">
@@ -2796,16 +2917,16 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15" customHeight="1">
@@ -2815,16 +2936,16 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15" customHeight="1">
@@ -2834,16 +2955,16 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1">
@@ -2853,16 +2974,16 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15" customHeight="1">
@@ -2872,16 +2993,16 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15" customHeight="1">
@@ -2891,16 +3012,16 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="15" customHeight="1">
@@ -2910,16 +3031,16 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="15" customHeight="1">
@@ -2929,16 +3050,16 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15" customHeight="1">
@@ -2948,16 +3069,16 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15" customHeight="1">
@@ -2967,16 +3088,16 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="15" customHeight="1">
@@ -2986,16 +3107,16 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="15" customHeight="1">
@@ -3005,16 +3126,16 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="15" customHeight="1">
@@ -3024,16 +3145,16 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="15" customHeight="1">
@@ -3043,16 +3164,16 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="15" customHeight="1">
@@ -3062,16 +3183,16 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="15" customHeight="1">
@@ -3081,16 +3202,16 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="15" customHeight="1">
@@ -3100,16 +3221,16 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="15" customHeight="1">
@@ -3119,16 +3240,16 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="15" customHeight="1">
@@ -3138,16 +3259,16 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="15" customHeight="1">
@@ -3157,16 +3278,16 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="15" customHeight="1">
@@ -3176,16 +3297,16 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="15" customHeight="1">
@@ -3195,16 +3316,16 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="15" customHeight="1">
@@ -3214,16 +3335,16 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="15" customHeight="1">
@@ -3233,16 +3354,16 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="15" customHeight="1">
@@ -3252,16 +3373,16 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="15" customHeight="1">
@@ -3271,16 +3392,16 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="2:8" ht="15" customHeight="1">
@@ -3290,16 +3411,16 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="15" customHeight="1">
@@ -3309,16 +3430,16 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="15" customHeight="1">
@@ -3328,16 +3449,16 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="15" customHeight="1">
@@ -3347,16 +3468,16 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="15" customHeight="1">
@@ -3366,16 +3487,16 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="63" spans="2:8" ht="15" customHeight="1">
@@ -3385,16 +3506,16 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="15" customHeight="1">
@@ -3404,533 +3525,546 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" ht="15" customHeight="1">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" customHeight="1">
       <c r="B65" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" ht="15" customHeight="1">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1">
       <c r="B66" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" ht="15" customHeight="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15" customHeight="1">
       <c r="B67" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" ht="15" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1">
       <c r="B68" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" ht="15" customHeight="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15" customHeight="1">
       <c r="B69" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" ht="15" customHeight="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15" customHeight="1">
       <c r="B70" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" ht="15" customHeight="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15" customHeight="1">
       <c r="B71" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" ht="15" customHeight="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15" customHeight="1">
       <c r="B72" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" ht="15" customHeight="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15" customHeight="1">
       <c r="B73" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" ht="15" customHeight="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15" customHeight="1">
       <c r="B74" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" ht="15" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1">
       <c r="B75" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" ht="15" customHeight="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1">
       <c r="B76" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" ht="15" customHeight="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15" customHeight="1">
       <c r="B77" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" ht="15" customHeight="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" customHeight="1">
       <c r="B78" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" ht="15" customHeight="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15" customHeight="1">
       <c r="B79" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" ht="15" customHeight="1">
-      <c r="B80" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15" customHeight="1">
+      <c r="A80" s="9"/>
+      <c r="B80" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" ht="15" customHeight="1">
-      <c r="B81" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15" customHeight="1">
+      <c r="A81" s="9"/>
+      <c r="B81" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" ht="15" customHeight="1">
-      <c r="B82" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" customHeight="1">
+      <c r="A82" s="9"/>
+      <c r="B82" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" ht="15" customHeight="1">
-      <c r="B83" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15" customHeight="1">
+      <c r="A83" s="9"/>
+      <c r="B83" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H83" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="F83" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="H83" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" ht="15" customHeight="1">
-      <c r="B84" s="7" t="s">
+    </row>
+    <row r="84" spans="1:8" ht="15" customHeight="1">
+      <c r="A84" s="9"/>
+      <c r="B84" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="H84" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="F84" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="H84" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" ht="15" customHeight="1">
-      <c r="B85" s="7" t="s">
+    </row>
+    <row r="85" spans="1:8" ht="15" customHeight="1">
+      <c r="A85" s="9"/>
+      <c r="B85" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="H85" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="F85" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="G85" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="H85" s="14" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" ht="15" customHeight="1">
-      <c r="B86" s="7" t="s">
+    </row>
+    <row r="86" spans="1:8" ht="15" customHeight="1">
+      <c r="A86" s="9"/>
+      <c r="B86" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H86" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F86" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" ht="15" customHeight="1">
-      <c r="B87" s="7" t="s">
+    </row>
+    <row r="87" spans="1:8" ht="15" customHeight="1">
+      <c r="A87" s="9"/>
+      <c r="B87" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="H87" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" ht="15" customHeight="1">
-      <c r="B88" s="7" t="s">
+    </row>
+    <row r="88" spans="1:8" ht="15" customHeight="1">
+      <c r="A88" s="9"/>
+      <c r="B88" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" ht="15" customHeight="1">
-      <c r="B89" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15" customHeight="1">
+      <c r="A89" s="9"/>
+      <c r="B89" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" ht="15" customHeight="1">
-      <c r="B90" s="7" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15" customHeight="1">
+      <c r="A90" s="9"/>
+      <c r="B90" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" ht="15" customHeight="1">
-      <c r="B91" s="7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15" customHeight="1">
+      <c r="A91" s="9"/>
+      <c r="B91" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" ht="15" customHeight="1">
-      <c r="B92" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15" customHeight="1">
+      <c r="A92" s="9"/>
+      <c r="B92" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C92" s="1"/>
@@ -3948,8 +4082,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="2:8" ht="15" customHeight="1">
-      <c r="B93" s="8" t="s">
+    <row r="93" spans="1:8" ht="15" customHeight="1">
+      <c r="A93" s="9"/>
+      <c r="B93" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C93" s="10"/>
@@ -3958,17 +4093,18 @@
         <v>23</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" ht="15" customHeight="1">
-      <c r="B94" s="9"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15" customHeight="1">
+      <c r="A94" s="9"/>
+      <c r="B94" s="18"/>
       <c r="C94" s="15" t="s">
         <v>17</v>
       </c>
@@ -3983,89 +4119,123 @@
         <v>29</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" ht="15" customHeight="1">
-      <c r="B95" s="9"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15" customHeight="1">
+      <c r="A95" s="9"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F95" s="1" t="s">
+      <c r="F95" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G95" s="1" t="s">
+      <c r="G95" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H95" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" ht="15" customHeight="1">
-      <c r="E96" s="2"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
-    </row>
-    <row r="97" spans="5:8" ht="15" customHeight="1">
-      <c r="E97" s="2"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-    </row>
-    <row r="98" spans="5:8" ht="15" customHeight="1">
-      <c r="E98" s="2"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-    </row>
-    <row r="99" spans="5:8" ht="15" customHeight="1">
+      <c r="H95" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="B96" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F96" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="B97" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="F97" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="G97" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="B98" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="F98" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="G98" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="15" customHeight="1">
       <c r="E99" s="2"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="6"/>
     </row>
-    <row r="100" spans="5:8" ht="15" customHeight="1">
+    <row r="100" spans="2:8" ht="15" customHeight="1">
       <c r="E100" s="2"/>
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
       <c r="H100" s="6"/>
     </row>
-    <row r="101" spans="5:8" ht="15" customHeight="1">
+    <row r="101" spans="2:8" ht="15" customHeight="1">
       <c r="E101" s="2"/>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
       <c r="H101" s="6"/>
     </row>
-    <row r="102" spans="5:8" ht="15" customHeight="1">
+    <row r="102" spans="2:8" ht="15" customHeight="1">
       <c r="E102" s="2"/>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
     </row>
-    <row r="103" spans="5:8" ht="15" customHeight="1">
+    <row r="103" spans="2:8" ht="15" customHeight="1">
       <c r="E103" s="2"/>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
     </row>
-    <row r="104" spans="5:8" ht="15" customHeight="1">
+    <row r="104" spans="2:8" ht="15" customHeight="1">
       <c r="E104" s="2"/>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
       <c r="H104" s="6"/>
     </row>
-    <row r="105" spans="5:8" ht="15" customHeight="1">
+    <row r="105" spans="2:8" ht="15" customHeight="1">
       <c r="E105" s="2"/>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
     </row>
-    <row r="106" spans="5:8" ht="15" customHeight="1">
+    <row r="106" spans="2:8" ht="15" customHeight="1">
       <c r="E106" s="2"/>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -4078,18 +4248,30 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:AA913">
-        <filterColumn colId="3">
-          <filters>
-            <filter val="V"/>
-          </filters>
-        </filterColumn>
-      </autoFilter>
+      <autoFilter ref="E1:E907"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="A2:I613"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <autoFilter ref="A1:N612"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -4110,68 +4292,76 @@
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{A49D9809-A3E9-4FA2-8EA4-867396B6504A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8ECEFC75-0BA8-4E9D-B916-608021674B63}" filter="1" showAutoFilter="1">
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A1:N612"/>
+      <autoFilter ref="A2:AA913">
+        <filterColumn colId="3">
+          <filters>
+            <filter val="V"/>
+          </filters>
+        </filterColumn>
+      </autoFilter>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2032162165"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{38507902-7545-485C-834F-5E4850BE1025}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="A2:I613"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2063878908"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{D250C68A-1DD9-40FD-B45F-2D5104E4B2FD}" filter="1" showAutoFilter="1">
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <autoFilter ref="E1:E907"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="573770298"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1007846334"/>
         </ext>
       </extLst>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="F2:H3 E1:E3 E96:E106 E4:H4 E92:H95">
-    <cfRule type="expression" dxfId="6" priority="85">
+  <conditionalFormatting sqref="F2:H3 E1:E3 E96 E4:H4 E92:H95 E99:E106">
+    <cfRule type="expression" dxfId="10" priority="89">
       <formula>COUNTIF($E:$E,$E1)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4 F1:F4 F92:F106 H92:H106">
-    <cfRule type="expression" dxfId="5" priority="86">
+  <conditionalFormatting sqref="H2:H4 F1:F4 F92:F96 H92:H96 H99:H106 F99:F106">
+    <cfRule type="expression" dxfId="9" priority="90">
       <formula>COUNTIF($F:$F,$F1)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:H87 E5:H19 E21:H83">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>COUNTIF($M:$M,$M5)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G68:G69 H85:H91 H5:H60 F85:F91 F5:F60 F62:F65 H62:H65 H67:H70 F67:F70 F73:F83 H73:H83">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>COUNTIF($N:$N,$N5)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58:G60">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>COUNTIF(#REF!,#REF!)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(E82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F88:H91 F20:H20">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>COUNTIF($M:$M,#REF!)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E97">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>COUNTIF($E:$E,$E97)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H97 F97:G98">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>COUNTIF($F:$F,$F97)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E98">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>COUNTIF($E:$E,$E98)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H98">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>COUNTIF($F:$F,$F98)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4180,17 +4370,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097749175EA382F46998456ACE2E5E022" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f9564bd998978afe117d271aa86623d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="656db63e-0aa2-4982-a6ef-7cfc894502dc" xmlns:ns3="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c8d268a87e81341ebbd7ca6aba28788" ns2:_="" ns3:_="">
     <xsd:import namespace="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
@@ -4401,6 +4580,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="656db63e-0aa2-4982-a6ef-7cfc894502dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4411,17 +4601,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
-    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B5B63AB-5528-472F-BE4A-13B18B02B409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4440,6 +4619,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{272F5C3E-8BC0-4DF6-913A-B867BEBD80EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a874f0ba-44be-4b2a-98a4-eb9ea6f4d70e"/>
+    <ds:schemaRef ds:uri="656db63e-0aa2-4982-a6ef-7cfc894502dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{043FBB36-7F63-4B63-8343-64EBAA2E147B}">
   <ds:schemaRefs>

</xml_diff>